<commit_message>
One cell modified (D1215)
</commit_message>
<xml_diff>
--- a/D1215.xlsx
+++ b/D1215.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farshad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farshad\Desktop\Git repos\Structural_Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513508B6-622B-4DCC-8A97-8992F92BE15A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC2BA7A-3CA9-44AE-A537-4799DA27A5BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,18 +76,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,15 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="P599" sqref="P599"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4754,28 +4745,28 @@
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="3">
+      <c r="A114" s="2">
         <v>113</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="2">
         <v>-15282.737999999999</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C114" s="2">
         <v>-1.4490000000000001</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="2">
         <v>-590.50300000000004</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E114" s="2">
         <v>6.3250000000000002</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F114" s="2">
         <v>1.7350000000000001</v>
       </c>
-      <c r="G114" s="3">
-        <v>0</v>
-      </c>
-      <c r="H114" s="3">
+      <c r="G114" s="2">
+        <v>0</v>
+      </c>
+      <c r="H114" s="2">
         <v>1</v>
       </c>
       <c r="I114" s="2">

</xml_diff>